<commit_message>
my work status on 22.04.14
</commit_message>
<xml_diff>
--- a/Docs/reports/Report.xlsx
+++ b/Docs/reports/Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -46,13 +46,16 @@
   </si>
   <si>
     <t>1. Написав першу робочу версію ServiceRefresh 2.Налаштував разом з Санею К. Realm Security на проді, тепере авторизація працює і там       3.Вбив 2,5 год. щоб залити собі репозиторій, зі своїм мобільним інтернетом(знаю, сам винний, що поїхав додому)</t>
+  </si>
+  <si>
+    <t>1.Війна з ajax, який постійно і нагло викидує Ajax error 2.Розробка CSE Dashboard (його готовність на перерішній час складає 7%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,10 +142,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -150,10 +152,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -244,7 +243,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -279,7 +277,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -455,111 +452,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:9" ht="225">
+      <c r="A2" s="6">
         <v>41747</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>41748</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="120">
+      <c r="A3" s="6">
+        <v>41751</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="1"/>
     </row>
   </sheetData>
@@ -569,24 +576,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
report 25.04 report problems
</commit_message>
<xml_diff>
--- a/Docs/reports/Report.xlsx
+++ b/Docs/reports/Report.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oksana\Documents\NetBeansProjects\InternetProviderWind\Docs\reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -91,11 +96,14 @@
   <si>
     <t>CSEdashboard - 12%      pagination - 32%</t>
   </si>
+  <si>
+    <t>CSEdashboard - 15%      pagination - 40%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -254,6 +262,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -585,11 +601,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -702,7 +718,9 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
+      <c r="H5" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="I5" s="11" t="s">
         <v>21</v>
       </c>
@@ -754,7 +772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -768,7 +786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Tasks and problems, report
</commit_message>
<xml_diff>
--- a/Docs/reports/Report.xlsx
+++ b/Docs/reports/Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -114,11 +114,17 @@
   <si>
     <t>CSEdashboard - 15%      pagination &amp; paging- 40%  done problems with server</t>
   </si>
+  <si>
+    <t>e2e, service order creating (map)- 40%</t>
+  </si>
+  <si>
+    <t>e2e, service order creating (map)- 60%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -619,19 +625,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="9" width="20.6640625" customWidth="1"/>
+    <col min="4" max="9" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -663,7 +669,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="135">
+    <row r="2" spans="1:9" ht="129.6">
       <c r="A2" s="3">
         <v>41747</v>
       </c>
@@ -678,7 +684,7 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="90">
+    <row r="3" spans="1:9" ht="86.4">
       <c r="A3" s="3">
         <v>41751</v>
       </c>
@@ -693,7 +699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="105">
+    <row r="4" spans="1:9" ht="100.8">
       <c r="A4" s="5">
         <v>41753</v>
       </c>
@@ -720,7 +726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30">
+    <row r="5" spans="1:9" ht="28.8">
       <c r="A5" s="9">
         <v>41754</v>
       </c>
@@ -733,7 +739,9 @@
       <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
         <v>24</v>
@@ -758,7 +766,9 @@
       <c r="D6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12" t="s">
         <v>26</v>
@@ -814,12 +824,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.69861111111111096" right="0.69861111111111096" top="0.75" bottom="0.75" header="0.29930555555555599" footer="0.29930555555555599"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -828,12 +838,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.69861111111111096" right="0.69861111111111096" top="0.75" bottom="0.75" header="0.29930555555555599" footer="0.29930555555555599"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>